<commit_message>
add data for task3
</commit_message>
<xml_diff>
--- a/assessment2/assessment2_calcs.xlsx
+++ b/assessment2/assessment2_calcs.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amanj\ds_projects\unsw\decision_making_6510\assessment2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B162B9B-49F8-4F98-BC52-ED87C5199CBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF6AE010-96DA-40D0-AC39-B2033CA61BD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" activeTab="1" xr2:uid="{128E22E7-D79F-4F4A-B9D4-5EF7FF588309}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" activeTab="2" xr2:uid="{128E22E7-D79F-4F4A-B9D4-5EF7FF588309}"/>
   </bookViews>
   <sheets>
     <sheet name="Task1" sheetId="1" r:id="rId1"/>
     <sheet name="Task2" sheetId="2" r:id="rId2"/>
-    <sheet name="Task3" sheetId="3" r:id="rId3"/>
+    <sheet name="Task3 - Data" sheetId="4" r:id="rId3"/>
+    <sheet name="Task3 - Analysis" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="TreeData" localSheetId="0">Task1!$ALM$1003:$ALT$1017</definedName>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -65,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="110">
   <si>
     <t>ID</t>
   </si>
@@ -148,9 +149,6 @@
     <t>Size of Site</t>
   </si>
   <si>
-    <t>Car-parking Facilities</t>
-  </si>
-  <si>
     <t>Visibility</t>
   </si>
   <si>
@@ -217,9 +215,6 @@
     <t>Size</t>
   </si>
   <si>
-    <t>Car-Parking</t>
-  </si>
-  <si>
     <t>Raw Weight</t>
   </si>
   <si>
@@ -259,22 +254,161 @@
     <t>1: Size of Site</t>
   </si>
   <si>
-    <t>2: Car-Parking</t>
+    <t>3: Closeness</t>
   </si>
   <si>
-    <t>3: Closeness</t>
+    <t>Car Parking</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
+  </si>
+  <si>
+    <t>2: Car Parking</t>
+  </si>
+  <si>
+    <t>Car Parking Facilities</t>
+  </si>
+  <si>
+    <t>TASK 3 - Data on Shortlisted Locations</t>
+  </si>
+  <si>
+    <t>Locations</t>
+  </si>
+  <si>
+    <t>Node ID</t>
+  </si>
+  <si>
+    <t>Latitude</t>
+  </si>
+  <si>
+    <t>Longitude</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Suburb</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>cnr Lygon St, Princes St</t>
+  </si>
+  <si>
+    <t>Carlton Nth</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>cnr Springvale Rd, Police Rd, Princes Hwy</t>
+  </si>
+  <si>
+    <t>Springvale</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>cnr Wellington Rd, Berwick Rd</t>
+  </si>
+  <si>
+    <t>Belgrave Sth</t>
+  </si>
+  <si>
+    <t>cnr Boundary Rd, Derrimut Rd</t>
+  </si>
+  <si>
+    <t>Derrimut</t>
+  </si>
+  <si>
+    <t>cnr Canning St, Richardson St</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>cnr Nepean Hwy, Warrigal Rd</t>
+  </si>
+  <si>
+    <t>Mentone</t>
+  </si>
+  <si>
+    <t>Accidents</t>
+  </si>
+  <si>
+    <t>Proximity to Vulnerable Populations</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Fatal</t>
+  </si>
+  <si>
+    <t>Serious</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>School</t>
+  </si>
+  <si>
+    <t>Hospital</t>
+  </si>
+  <si>
+    <t>Aged Care</t>
+  </si>
+  <si>
+    <t>Peak-Hour Congestion</t>
+  </si>
+  <si>
+    <t>Local Population</t>
+  </si>
+  <si>
+    <t>Congestion Factor</t>
+  </si>
+  <si>
+    <t>LGA</t>
+  </si>
+  <si>
+    <t>Population</t>
+  </si>
+  <si>
+    <t>borders Yarra and Melbourne</t>
+  </si>
+  <si>
+    <t>borders Monash and Greater Dandenong</t>
+  </si>
+  <si>
+    <t>Yarra Ranges</t>
+  </si>
+  <si>
+    <t>borders Wyndham and Melton</t>
+  </si>
+  <si>
+    <t>Yarra</t>
+  </si>
+  <si>
+    <t>Kingston</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0_ ;\-0\ "/>
+    <numFmt numFmtId="166" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -297,6 +431,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -306,7 +448,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="36">
     <border>
       <left/>
       <right/>
@@ -394,12 +536,329 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -428,16 +887,104 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="12" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
+    <xf numFmtId="18" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="18" fontId="1" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="18" fontId="1" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="18" fontId="1" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -571,7 +1118,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FBB962CD-2968-48FC-9CBF-ABEF3EEEC9FC}" type="CELLRANGE">
+                    <a:fld id="{FC93CA7E-0DC3-4338-9F38-13E217806D04}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -610,7 +1157,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{79B85AC4-CF6F-4385-B26E-1A371D71A938}" type="CELLRANGE">
+                    <a:fld id="{829772F3-B7BE-483A-B9E2-BBA650A4AC31}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -649,7 +1196,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9D9C0C95-2343-4955-8A38-C1C896CBE874}" type="CELLRANGE">
+                    <a:fld id="{C44E87FA-56AF-4F98-B939-17647B783E1A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -688,7 +1235,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6C7E001F-CF7A-4EE2-AFC1-CEEA1188A60A}" type="CELLRANGE">
+                    <a:fld id="{F8FEEE36-DC27-47B7-BD95-7080C61A77A5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -727,7 +1274,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1C0BAB4B-32E8-4EF5-9BA8-D9934579C982}" type="CELLRANGE">
+                    <a:fld id="{6D627C65-670F-43BC-BFD8-A33B1844BBDF}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2340,7 +2887,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-AU" baseline="0"/>
-              <a:t> Value vs Weight of Car-Parking Attribute</a:t>
+              <a:t> Value vs Weight of Car Parking Attribute</a:t>
             </a:r>
             <a:endParaRPr lang="en-AU"/>
           </a:p>
@@ -3088,7 +3635,7 @@
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-AU" baseline="0"/>
-                  <a:t> Car-Parking Attribute</a:t>
+                  <a:t> Car Parking Attribute</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-AU"/>
               </a:p>
@@ -9915,7 +10462,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -9928,7 +10475,9 @@
   </sheetPr>
   <dimension ref="A1:ALT1017"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -9948,8 +10497,8 @@
     <col min="2000" max="2000" width="2.4140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:19" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A1" s="20" t="s">
         <v>23</v>
       </c>
     </row>
@@ -10675,8 +11224,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3004556E-934C-4078-9F8A-DC164B820FA9}">
   <dimension ref="A1:N145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A161" workbookViewId="0">
-      <selection activeCell="B171" sqref="B171"/>
+    <sheetView topLeftCell="A168" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -10690,8 +11239,8 @@
     <col min="2000" max="2000" width="2.4140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A1" s="20" t="s">
         <v>24</v>
       </c>
     </row>
@@ -10700,21 +11249,21 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B5" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B6" s="11"/>
       <c r="C6" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="12" t="s">
         <v>37</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
@@ -10743,7 +11292,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
-        <v>27</v>
+        <v>67</v>
       </c>
       <c r="C9">
         <v>90</v>
@@ -10755,7 +11304,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C10">
         <v>10</v>
@@ -10767,7 +11316,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C11">
         <v>40</v>
@@ -10779,24 +11328,24 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B13" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C15" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="12" t="s">
+      <c r="E15" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="E15" s="12" t="s">
+      <c r="F15" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="F15" s="12" t="s">
+      <c r="G15" s="12" t="s">
         <v>35</v>
-      </c>
-      <c r="G15" s="12" t="s">
-        <v>36</v>
       </c>
       <c r="H15" s="15"/>
     </row>
@@ -10842,7 +11391,7 @@
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
-        <v>27</v>
+        <v>67</v>
       </c>
       <c r="C18">
         <v>80</v>
@@ -10862,7 +11411,7 @@
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C19">
         <v>100</v>
@@ -10882,7 +11431,7 @@
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C20">
         <v>50</v>
@@ -10902,7 +11451,7 @@
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B21" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C21" s="13">
         <f>SUMPRODUCT(C16:C20,$D$7:$D$11)/100</f>
@@ -10927,26 +11476,26 @@
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B23" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.35">
       <c r="C25" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D25" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="D25" s="12" t="s">
-        <v>44</v>
-      </c>
       <c r="E25" s="12" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F25" s="15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C26" s="16">
         <v>105000</v>
@@ -10964,7 +11513,7 @@
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C27" s="16">
         <v>60000</v>
@@ -10984,7 +11533,7 @@
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B28" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C28" s="16">
         <v>35000</v>
@@ -11000,11 +11549,11 @@
         <v>125000</v>
       </c>
       <c r="J28" s="12"/>
-      <c r="K28" s="18"/>
+      <c r="K28" s="12"/>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C29" s="16">
         <v>75000</v>
@@ -11019,12 +11568,12 @@
         <f t="shared" si="2"/>
         <v>130000</v>
       </c>
-      <c r="J29" s="19"/>
+      <c r="J29" s="18"/>
       <c r="K29" s="12"/>
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B30" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C30" s="16">
         <v>90000</v>
@@ -11042,89 +11591,83 @@
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B32" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J32" s="12"/>
       <c r="K32" s="12"/>
     </row>
     <row r="33" spans="10:11" x14ac:dyDescent="0.35">
       <c r="J33" s="12"/>
-      <c r="K33" s="18"/>
+      <c r="K33" s="12"/>
     </row>
     <row r="34" spans="10:11" x14ac:dyDescent="0.35">
-      <c r="J34" s="19"/>
+      <c r="J34" s="18"/>
       <c r="K34" s="12"/>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A57" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="I57" s="21"/>
-      <c r="J57" s="21"/>
-      <c r="K57" s="21"/>
+        <v>60</v>
+      </c>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A58" s="11"/>
-      <c r="I58" s="21"/>
-      <c r="J58" s="21"/>
-      <c r="K58" s="21"/>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A59" s="11"/>
       <c r="B59" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="E59" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="F59" s="20"/>
-      <c r="G59" s="20"/>
-      <c r="H59" s="20"/>
-      <c r="I59" s="20"/>
-      <c r="J59" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="K59" s="20"/>
-      <c r="L59" s="20"/>
-      <c r="M59" s="20"/>
-      <c r="N59" s="20"/>
+        <v>61</v>
+      </c>
+      <c r="E59" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="F59" s="19"/>
+      <c r="G59" s="19"/>
+      <c r="H59" s="19"/>
+      <c r="I59" s="19"/>
+      <c r="J59" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="K59" s="19"/>
+      <c r="L59" s="19"/>
+      <c r="M59" s="19"/>
+      <c r="N59" s="19"/>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.35">
       <c r="C60" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="D60" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="E60" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="F60" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="G60" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="H60" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="I60" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="D60" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="E60" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="F60" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="G60" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="H60" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="I60" s="12" t="s">
-        <v>53</v>
-      </c>
       <c r="J60" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="K60" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="L60" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="K60" s="12" t="s">
+      <c r="M60" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="L60" s="12" t="s">
+      <c r="N60" s="12" t="s">
         <v>58</v>
-      </c>
-      <c r="M60" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="N60" s="12" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.35">
@@ -11668,59 +12211,59 @@
     </row>
     <row r="96" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B96" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="E96" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="F96" s="20"/>
-      <c r="G96" s="20"/>
-      <c r="H96" s="20"/>
-      <c r="I96" s="20"/>
-      <c r="J96" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="K96" s="20"/>
-      <c r="L96" s="20"/>
-      <c r="M96" s="20"/>
-      <c r="N96" s="20"/>
+        <v>66</v>
+      </c>
+      <c r="E96" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="F96" s="19"/>
+      <c r="G96" s="19"/>
+      <c r="H96" s="19"/>
+      <c r="I96" s="19"/>
+      <c r="J96" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="K96" s="19"/>
+      <c r="L96" s="19"/>
+      <c r="M96" s="19"/>
+      <c r="N96" s="19"/>
     </row>
     <row r="97" spans="3:14" x14ac:dyDescent="0.35">
       <c r="C97" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="D97" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="E97" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="F97" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="G97" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="H97" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="I97" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="D97" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="E97" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="F97" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="G97" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="H97" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="I97" s="12" t="s">
-        <v>53</v>
-      </c>
       <c r="J97" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="K97" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="L97" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="K97" s="12" t="s">
+      <c r="M97" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="L97" s="12" t="s">
+      <c r="N97" s="12" t="s">
         <v>58</v>
-      </c>
-      <c r="M97" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="N97" s="12" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="98" spans="3:14" x14ac:dyDescent="0.35">
@@ -12489,7 +13032,9 @@
       <c r="F126" s="14"/>
       <c r="G126" s="14"/>
       <c r="H126" s="14"/>
-      <c r="I126" s="14"/>
+      <c r="I126" s="14" t="s">
+        <v>65</v>
+      </c>
       <c r="J126" s="13"/>
       <c r="K126" s="13"/>
       <c r="L126" s="13"/>
@@ -12528,7 +13073,9 @@
       <c r="F129" s="14"/>
       <c r="G129" s="14"/>
       <c r="H129" s="14"/>
-      <c r="I129" s="14"/>
+      <c r="I129" s="14" t="s">
+        <v>64</v>
+      </c>
       <c r="J129" s="13"/>
       <c r="K129" s="13"/>
       <c r="L129" s="13"/>
@@ -12576,59 +13123,59 @@
     </row>
     <row r="133" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B133" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="E133" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="F133" s="20"/>
-      <c r="G133" s="20"/>
-      <c r="H133" s="20"/>
-      <c r="I133" s="20"/>
-      <c r="J133" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="K133" s="20"/>
-      <c r="L133" s="20"/>
-      <c r="M133" s="20"/>
-      <c r="N133" s="20"/>
+        <v>62</v>
+      </c>
+      <c r="E133" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="F133" s="19"/>
+      <c r="G133" s="19"/>
+      <c r="H133" s="19"/>
+      <c r="I133" s="19"/>
+      <c r="J133" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="K133" s="19"/>
+      <c r="L133" s="19"/>
+      <c r="M133" s="19"/>
+      <c r="N133" s="19"/>
     </row>
     <row r="134" spans="2:14" x14ac:dyDescent="0.35">
       <c r="C134" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="D134" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="E134" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="F134" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="G134" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="H134" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="I134" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="D134" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="E134" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="F134" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="G134" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="H134" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="I134" s="12" t="s">
-        <v>53</v>
-      </c>
       <c r="J134" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="K134" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="L134" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="K134" s="12" t="s">
+      <c r="M134" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="L134" s="12" t="s">
+      <c r="N134" s="12" t="s">
         <v>58</v>
-      </c>
-      <c r="M134" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="N134" s="12" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="135" spans="2:14" x14ac:dyDescent="0.35">
@@ -13186,6 +13733,649 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31FDB724-EB94-4F12-9560-B4EA39B854DF}">
+  <dimension ref="A1:R32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="4.75" customWidth="1"/>
+    <col min="3" max="3" width="7.83203125" customWidth="1"/>
+    <col min="4" max="4" width="8.6640625" customWidth="1"/>
+    <col min="5" max="5" width="10" customWidth="1"/>
+    <col min="6" max="6" width="9.33203125" customWidth="1"/>
+    <col min="7" max="7" width="11.4140625" customWidth="1"/>
+    <col min="8" max="8" width="5.5" customWidth="1"/>
+    <col min="9" max="9" width="8.25" customWidth="1"/>
+    <col min="10" max="10" width="11.25" customWidth="1"/>
+    <col min="11" max="11" width="9.83203125" customWidth="1"/>
+    <col min="12" max="12" width="5.83203125" customWidth="1"/>
+    <col min="13" max="13" width="10.6640625" customWidth="1"/>
+    <col min="14" max="14" width="7" customWidth="1"/>
+    <col min="15" max="15" width="10.25" customWidth="1"/>
+    <col min="16" max="16" width="9.25" customWidth="1"/>
+    <col min="17" max="17" width="9.6640625" customWidth="1"/>
+    <col min="18" max="18" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="35" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A1" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" s="20"/>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="B2" s="11"/>
+      <c r="R2" s="13"/>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="B3" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="R3" s="13"/>
+    </row>
+    <row r="4" spans="1:18" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B4" s="11"/>
+      <c r="R4" s="13"/>
+    </row>
+    <row r="5" spans="1:18" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C5" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="D5" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="E5" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="F5" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="G5" s="25"/>
+      <c r="H5" s="25"/>
+      <c r="I5" s="26"/>
+      <c r="J5" s="23" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="B6" s="27" t="s">
+        <v>75</v>
+      </c>
+      <c r="C6" s="28">
+        <v>36335</v>
+      </c>
+      <c r="D6" s="29">
+        <v>-37.792262218399998</v>
+      </c>
+      <c r="E6" s="30">
+        <v>144.96841020839997</v>
+      </c>
+      <c r="F6" s="31" t="s">
+        <v>76</v>
+      </c>
+      <c r="G6" s="32"/>
+      <c r="H6" s="32"/>
+      <c r="I6" s="33"/>
+      <c r="J6" s="34" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="B7" s="35" t="s">
+        <v>78</v>
+      </c>
+      <c r="C7" s="36">
+        <v>10592</v>
+      </c>
+      <c r="D7" s="37">
+        <v>-37.933161954347831</v>
+      </c>
+      <c r="E7" s="38">
+        <v>145.15677819478265</v>
+      </c>
+      <c r="F7" s="39" t="s">
+        <v>79</v>
+      </c>
+      <c r="G7" s="40"/>
+      <c r="H7" s="40"/>
+      <c r="I7" s="41"/>
+      <c r="J7" s="42" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="B8" s="35" t="s">
+        <v>81</v>
+      </c>
+      <c r="C8" s="36">
+        <v>42680</v>
+      </c>
+      <c r="D8" s="37">
+        <v>-37.961190742608693</v>
+      </c>
+      <c r="E8" s="38">
+        <v>145.36115421347824</v>
+      </c>
+      <c r="F8" s="39" t="s">
+        <v>82</v>
+      </c>
+      <c r="G8" s="40"/>
+      <c r="H8" s="40"/>
+      <c r="I8" s="41"/>
+      <c r="J8" s="42" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="B9" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="36">
+        <v>45524</v>
+      </c>
+      <c r="D9" s="37">
+        <v>-37.805022546363631</v>
+      </c>
+      <c r="E9" s="38">
+        <v>144.69593451409091</v>
+      </c>
+      <c r="F9" s="39" t="s">
+        <v>84</v>
+      </c>
+      <c r="G9" s="40"/>
+      <c r="H9" s="40"/>
+      <c r="I9" s="41"/>
+      <c r="J9" s="42" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="B10" s="35" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="36">
+        <v>29361</v>
+      </c>
+      <c r="D10" s="37">
+        <v>-37.784910360476204</v>
+      </c>
+      <c r="E10" s="38">
+        <v>144.97506995476192</v>
+      </c>
+      <c r="F10" s="39" t="s">
+        <v>86</v>
+      </c>
+      <c r="G10" s="40"/>
+      <c r="H10" s="40"/>
+      <c r="I10" s="41"/>
+      <c r="J10" s="42" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B11" s="43" t="s">
+        <v>87</v>
+      </c>
+      <c r="C11" s="44">
+        <v>35605</v>
+      </c>
+      <c r="D11" s="45">
+        <v>-37.98216354238096</v>
+      </c>
+      <c r="E11" s="46">
+        <v>145.07139516952378</v>
+      </c>
+      <c r="F11" s="47" t="s">
+        <v>88</v>
+      </c>
+      <c r="G11" s="48"/>
+      <c r="H11" s="48"/>
+      <c r="I11" s="49"/>
+      <c r="J11" s="50" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="B12" s="11"/>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="B13" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="15" spans="1:18" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C15" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="D15" s="51" t="s">
+        <v>93</v>
+      </c>
+      <c r="E15" s="52" t="s">
+        <v>94</v>
+      </c>
+      <c r="F15" s="23" t="s">
+        <v>95</v>
+      </c>
+      <c r="G15" s="15"/>
+      <c r="I15" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="J15" s="52" t="s">
+        <v>97</v>
+      </c>
+      <c r="K15" s="23" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="B16" s="27" t="s">
+        <v>75</v>
+      </c>
+      <c r="C16" s="36">
+        <v>25</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16" s="53">
+        <v>10</v>
+      </c>
+      <c r="F16" s="42">
+        <v>15</v>
+      </c>
+      <c r="H16" s="27" t="s">
+        <v>75</v>
+      </c>
+      <c r="I16" s="54">
+        <v>0.6</v>
+      </c>
+      <c r="J16" s="53">
+        <v>1.9</v>
+      </c>
+      <c r="K16" s="42">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B17" s="35" t="s">
+        <v>78</v>
+      </c>
+      <c r="C17" s="36">
+        <v>23</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17" s="53">
+        <v>14</v>
+      </c>
+      <c r="F17" s="42">
+        <v>9</v>
+      </c>
+      <c r="H17" s="35" t="s">
+        <v>78</v>
+      </c>
+      <c r="I17" s="54">
+        <v>0.24</v>
+      </c>
+      <c r="J17" s="53">
+        <v>3.9</v>
+      </c>
+      <c r="K17" s="42">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B18" s="35" t="s">
+        <v>81</v>
+      </c>
+      <c r="C18" s="36">
+        <v>23</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18" s="53">
+        <v>9</v>
+      </c>
+      <c r="F18" s="42">
+        <v>13</v>
+      </c>
+      <c r="H18" s="35" t="s">
+        <v>81</v>
+      </c>
+      <c r="I18" s="54">
+        <v>2.8</v>
+      </c>
+      <c r="J18" s="53">
+        <v>12.9</v>
+      </c>
+      <c r="K18" s="42">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B19" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="36">
+        <v>22</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19" s="53">
+        <v>8</v>
+      </c>
+      <c r="F19" s="42">
+        <v>14</v>
+      </c>
+      <c r="H19" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="I19" s="54">
+        <v>3.2</v>
+      </c>
+      <c r="J19" s="53">
+        <v>6.6</v>
+      </c>
+      <c r="K19" s="42">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B20" s="35" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" s="36">
+        <v>21</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20" s="53">
+        <v>7</v>
+      </c>
+      <c r="F20" s="42">
+        <v>14</v>
+      </c>
+      <c r="H20" s="35" t="s">
+        <v>11</v>
+      </c>
+      <c r="I20" s="54">
+        <v>1</v>
+      </c>
+      <c r="J20" s="53">
+        <v>1.5</v>
+      </c>
+      <c r="K20" s="42">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="21" spans="2:13" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B21" s="43" t="s">
+        <v>87</v>
+      </c>
+      <c r="C21" s="44">
+        <v>21</v>
+      </c>
+      <c r="D21" s="55">
+        <v>0</v>
+      </c>
+      <c r="E21" s="56">
+        <v>9</v>
+      </c>
+      <c r="F21" s="50">
+        <v>12</v>
+      </c>
+      <c r="H21" s="43" t="s">
+        <v>87</v>
+      </c>
+      <c r="I21" s="57">
+        <v>0.16</v>
+      </c>
+      <c r="J21" s="56">
+        <v>2.8</v>
+      </c>
+      <c r="K21" s="50">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B23" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="H23" s="11" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="2:13" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="25" spans="2:13" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C25" s="58">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="D25" s="59">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="E25" s="60" t="s">
+        <v>101</v>
+      </c>
+      <c r="I25" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="J25" s="25"/>
+      <c r="K25" s="25"/>
+      <c r="L25" s="26"/>
+      <c r="M25" s="23" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="26" spans="2:13" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C26" s="61"/>
+      <c r="D26" s="62"/>
+      <c r="E26" s="63"/>
+      <c r="H26" s="27" t="s">
+        <v>75</v>
+      </c>
+      <c r="I26" s="31" t="s">
+        <v>104</v>
+      </c>
+      <c r="J26" s="32"/>
+      <c r="K26" s="32"/>
+      <c r="L26" s="33"/>
+      <c r="M26" s="34">
+        <f>103125+183756</f>
+        <v>286881</v>
+      </c>
+    </row>
+    <row r="27" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B27" s="27" t="s">
+        <v>75</v>
+      </c>
+      <c r="C27" s="54">
+        <v>2</v>
+      </c>
+      <c r="D27" s="53">
+        <v>9</v>
+      </c>
+      <c r="E27" s="64">
+        <f>D27/C27</f>
+        <v>4.5</v>
+      </c>
+      <c r="H27" s="35" t="s">
+        <v>78</v>
+      </c>
+      <c r="I27" s="39" t="s">
+        <v>105</v>
+      </c>
+      <c r="J27" s="40"/>
+      <c r="K27" s="40"/>
+      <c r="L27" s="41"/>
+      <c r="M27" s="42">
+        <f>204936+168362</f>
+        <v>373298</v>
+      </c>
+    </row>
+    <row r="28" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B28" s="35" t="s">
+        <v>78</v>
+      </c>
+      <c r="C28" s="54">
+        <v>2</v>
+      </c>
+      <c r="D28" s="53">
+        <v>3</v>
+      </c>
+      <c r="E28" s="64">
+        <f t="shared" ref="E28:E32" si="0">D28/C28</f>
+        <v>1.5</v>
+      </c>
+      <c r="H28" s="35" t="s">
+        <v>81</v>
+      </c>
+      <c r="I28" s="39" t="s">
+        <v>106</v>
+      </c>
+      <c r="J28" s="40"/>
+      <c r="K28" s="40"/>
+      <c r="L28" s="41"/>
+      <c r="M28" s="42">
+        <v>159955</v>
+      </c>
+    </row>
+    <row r="29" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B29" s="35" t="s">
+        <v>81</v>
+      </c>
+      <c r="C29" s="54">
+        <v>1</v>
+      </c>
+      <c r="D29" s="53">
+        <v>1</v>
+      </c>
+      <c r="E29" s="64">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H29" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="I29" s="39" t="s">
+        <v>107</v>
+      </c>
+      <c r="J29" s="40"/>
+      <c r="K29" s="40"/>
+      <c r="L29" s="41"/>
+      <c r="M29" s="42">
+        <f>283294+172500</f>
+        <v>455794</v>
+      </c>
+    </row>
+    <row r="30" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B30" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="C30" s="54">
+        <v>2</v>
+      </c>
+      <c r="D30" s="53">
+        <v>3</v>
+      </c>
+      <c r="E30" s="64">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+      <c r="H30" s="35" t="s">
+        <v>11</v>
+      </c>
+      <c r="I30" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="J30" s="40"/>
+      <c r="K30" s="40"/>
+      <c r="L30" s="41"/>
+      <c r="M30" s="42">
+        <v>103125</v>
+      </c>
+    </row>
+    <row r="31" spans="2:13" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B31" s="35" t="s">
+        <v>11</v>
+      </c>
+      <c r="C31" s="54">
+        <v>3</v>
+      </c>
+      <c r="D31" s="53">
+        <v>4</v>
+      </c>
+      <c r="E31" s="64">
+        <f t="shared" si="0"/>
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="H31" s="43" t="s">
+        <v>87</v>
+      </c>
+      <c r="I31" s="47" t="s">
+        <v>109</v>
+      </c>
+      <c r="J31" s="48"/>
+      <c r="K31" s="48"/>
+      <c r="L31" s="49"/>
+      <c r="M31" s="50">
+        <v>167293</v>
+      </c>
+    </row>
+    <row r="32" spans="2:13" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B32" s="43" t="s">
+        <v>87</v>
+      </c>
+      <c r="C32" s="57">
+        <v>2</v>
+      </c>
+      <c r="D32" s="56">
+        <v>3</v>
+      </c>
+      <c r="E32" s="65">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="17">
+    <mergeCell ref="I27:L27"/>
+    <mergeCell ref="I28:L28"/>
+    <mergeCell ref="I29:L29"/>
+    <mergeCell ref="I30:L30"/>
+    <mergeCell ref="I31:L31"/>
+    <mergeCell ref="F11:I11"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="I25:L25"/>
+    <mergeCell ref="I26:L26"/>
+    <mergeCell ref="F5:I5"/>
+    <mergeCell ref="F6:I6"/>
+    <mergeCell ref="F7:I7"/>
+    <mergeCell ref="F8:I8"/>
+    <mergeCell ref="F9:I9"/>
+    <mergeCell ref="F10:I10"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8779BE29-FEF8-4926-9FA0-B0F9F251FEB8}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
complete decision for task3
</commit_message>
<xml_diff>
--- a/assessment2/assessment2_calcs.xlsx
+++ b/assessment2/assessment2_calcs.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amanj\ds_projects\unsw\decision_making_6510\assessment2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EF4ACDF-CB3A-41AC-B60A-5A258D537BFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8EAC077-0D57-4ABC-A0A8-D41B26F6CA3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" activeTab="3" xr2:uid="{128E22E7-D79F-4F4A-B9D4-5EF7FF588309}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" tabRatio="730" activeTab="4" xr2:uid="{128E22E7-D79F-4F4A-B9D4-5EF7FF588309}"/>
   </bookViews>
   <sheets>
     <sheet name="Task1" sheetId="1" r:id="rId1"/>
     <sheet name="Task2" sheetId="2" r:id="rId2"/>
     <sheet name="Task3 - Raw Data" sheetId="4" r:id="rId3"/>
-    <sheet name="Task3 - Value Functions" sheetId="3" r:id="rId4"/>
-    <sheet name="Sheet2" sheetId="5" r:id="rId5"/>
+    <sheet name="Task3 - Value Funcs and Weights" sheetId="3" r:id="rId4"/>
+    <sheet name="Task3 - Analysis" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="TreeData" localSheetId="0">Task1!$ALM$1003:$ALT$1017</definedName>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="142">
   <si>
     <t>ID</t>
   </si>
@@ -378,6 +378,9 @@
     <t>LGA</t>
   </si>
   <si>
+    <t>Population</t>
+  </si>
+  <si>
     <t>borders Yarra and Melbourne</t>
   </si>
   <si>
@@ -405,6 +408,9 @@
     <t>Congestion</t>
   </si>
   <si>
+    <t>Proximity</t>
+  </si>
+  <si>
     <t>Cong.</t>
   </si>
   <si>
@@ -424,6 +430,9 @@
   </si>
   <si>
     <t>All Attributes</t>
+  </si>
+  <si>
+    <t>Sum</t>
   </si>
   <si>
     <t>Weighted Sum</t>
@@ -448,6 +457,42 @@
   </si>
   <si>
     <t>Sum of Weights</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Running Total</t>
+  </si>
+  <si>
+    <t>Count</t>
+  </si>
+  <si>
+    <t>Bottom-Level Attributes</t>
+  </si>
+  <si>
+    <t>Top-Level Attributes</t>
+  </si>
+  <si>
+    <t>Danger</t>
+  </si>
+  <si>
+    <t>Benefaction</t>
+  </si>
+  <si>
+    <t>Weight</t>
+  </si>
+  <si>
+    <t>Location with maximum exigency:</t>
+  </si>
+  <si>
+    <t>Evaluate performance of alternatives</t>
+  </si>
+  <si>
+    <t>Decision</t>
+  </si>
+  <si>
+    <t>Sensitivity Analysis</t>
   </si>
 </sst>
 </file>
@@ -1281,7 +1326,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{721CCC95-DFBB-4E43-BC83-9F8389CF1E59}" type="CELLRANGE">
+                    <a:fld id="{CC58A28B-D2A5-40BD-A882-2514FAA6A7EF}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1320,7 +1365,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DB142437-DEFB-4A93-85D8-EB06E9A18710}" type="CELLRANGE">
+                    <a:fld id="{3D78EAAD-E776-4141-93AF-828373D50EB3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1359,7 +1404,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5D390DF5-3582-4183-B6AC-6DF7F0F0D2FB}" type="CELLRANGE">
+                    <a:fld id="{A151F7FF-39EA-4454-A10C-380DE40F082D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1398,7 +1443,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1AAC3B8C-4DD0-426E-9663-5793CAEDDB83}" type="CELLRANGE">
+                    <a:fld id="{A707F285-9D91-4FBE-ADE7-D1A15F1BB751}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1437,7 +1482,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2A94C8F1-7143-4D74-958A-6825973D6D90}" type="CELLRANGE">
+                    <a:fld id="{A5BB738B-D4DC-4827-B6E7-E98118643C25}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5251,7 +5296,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Task3 - Value Functions'!$C$18:$C$22</c:f>
+              <c:f>'Task3 - Value Funcs and Weights'!$C$18:$C$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -5275,7 +5320,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Task3 - Value Functions'!$B$18:$B$22</c:f>
+              <c:f>'Task3 - Value Funcs and Weights'!$B$18:$B$22</c:f>
               <c:numCache>
                 <c:formatCode>#\ ?/?</c:formatCode>
                 <c:ptCount val="5"/>
@@ -5703,7 +5748,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Task3 - Value Functions'!$D$18:$D$22</c:f>
+              <c:f>'Task3 - Value Funcs and Weights'!$D$18:$D$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -5727,7 +5772,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Task3 - Value Functions'!$B$18:$B$22</c:f>
+              <c:f>'Task3 - Value Funcs and Weights'!$B$18:$B$22</c:f>
               <c:numCache>
                 <c:formatCode>#\ ?/?</c:formatCode>
                 <c:ptCount val="5"/>
@@ -6060,7 +6105,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Task3 - Value Functions'!$E$18:$E$22</c:f>
+              <c:f>'Task3 - Value Funcs and Weights'!$E$18:$E$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -6084,7 +6129,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Task3 - Value Functions'!$B$18:$B$22</c:f>
+              <c:f>'Task3 - Value Funcs and Weights'!$B$18:$B$22</c:f>
               <c:numCache>
                 <c:formatCode>#\ ?/?</c:formatCode>
                 <c:ptCount val="5"/>
@@ -6417,7 +6462,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Task3 - Value Functions'!$F$18:$F$22</c:f>
+              <c:f>'Task3 - Value Funcs and Weights'!$F$18:$F$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -6441,7 +6486,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Task3 - Value Functions'!$B$18:$B$22</c:f>
+              <c:f>'Task3 - Value Funcs and Weights'!$B$18:$B$22</c:f>
               <c:numCache>
                 <c:formatCode>#\ ?/?</c:formatCode>
                 <c:ptCount val="5"/>
@@ -6463,7 +6508,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="1"/>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-0730-421A-8DF9-C39724089A50}"/>
@@ -6784,7 +6829,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Task3 - Value Functions'!$G$18:$G$22</c:f>
+              <c:f>'Task3 - Value Funcs and Weights'!$G$18:$G$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -6808,7 +6853,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Task3 - Value Functions'!$B$18:$B$22</c:f>
+              <c:f>'Task3 - Value Funcs and Weights'!$B$18:$B$22</c:f>
               <c:numCache>
                 <c:formatCode>#\ ?/?</c:formatCode>
                 <c:ptCount val="5"/>
@@ -6830,7 +6875,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="1"/>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-5A02-4659-9C4B-C0E79345EBA2}"/>
@@ -12835,7 +12880,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>222250</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>41</xdr:row>
       <xdr:rowOff>136525</xdr:rowOff>
     </xdr:to>
@@ -12911,7 +12956,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>222250</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>60</xdr:row>
       <xdr:rowOff>136525</xdr:rowOff>
     </xdr:to>
@@ -12987,7 +13032,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>222250</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>79</xdr:row>
       <xdr:rowOff>136525</xdr:rowOff>
     </xdr:to>
@@ -14070,8 +14115,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3004556E-934C-4078-9F8A-DC164B820FA9}">
   <dimension ref="A1:N145"/>
   <sheetViews>
-    <sheetView topLeftCell="A81" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C173" sqref="C173"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -16582,8 +16627,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31FDB724-EB94-4F12-9560-B4EA39B854DF}">
   <dimension ref="A1:R32"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="M30" sqref="M30"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -17023,7 +17068,7 @@
       <c r="K25" s="90"/>
       <c r="L25" s="92"/>
       <c r="M25" s="60" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
     </row>
     <row r="26" spans="2:13" ht="16" thickBot="1" x14ac:dyDescent="0.4">
@@ -17054,7 +17099,7 @@
         <v>75</v>
       </c>
       <c r="I27" s="78" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="J27" s="79"/>
       <c r="K27" s="79"/>
@@ -17082,7 +17127,7 @@
         <v>78</v>
       </c>
       <c r="I28" s="81" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="J28" s="94"/>
       <c r="K28" s="94"/>
@@ -17110,7 +17155,7 @@
         <v>81</v>
       </c>
       <c r="I29" s="81" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="J29" s="94"/>
       <c r="K29" s="94"/>
@@ -17138,7 +17183,7 @@
         <v>9</v>
       </c>
       <c r="I30" s="81" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="J30" s="94"/>
       <c r="K30" s="94"/>
@@ -17166,7 +17211,7 @@
         <v>11</v>
       </c>
       <c r="I31" s="81" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="J31" s="94"/>
       <c r="K31" s="94"/>
@@ -17194,7 +17239,7 @@
         <v>87</v>
       </c>
       <c r="I32" s="83" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="J32" s="84"/>
       <c r="K32" s="84"/>
@@ -17226,16 +17271,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8779BE29-FEF8-4926-9FA0-B0F9F251FEB8}">
-  <dimension ref="A1:I89"/>
+  <dimension ref="A1:I98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
-      <selection activeCell="C94" sqref="C94"/>
+    <sheetView topLeftCell="A81" workbookViewId="0">
+      <selection activeCell="F98" sqref="F98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="2" width="6.83203125" customWidth="1"/>
-    <col min="3" max="3" width="9.4140625" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" customWidth="1"/>
     <col min="4" max="4" width="10.5" customWidth="1"/>
     <col min="5" max="5" width="11.1640625" customWidth="1"/>
     <col min="6" max="6" width="14.33203125" customWidth="1"/>
@@ -17247,18 +17292,18 @@
   <sheetData>
     <row r="1" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A1" s="20" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="B1" s="20"/>
     </row>
     <row r="3" spans="1:9" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="11" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="11" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="15.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
@@ -17273,10 +17318,10 @@
         <v>98</v>
       </c>
       <c r="F7" s="69" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="H7" s="68" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -17407,12 +17452,12 @@
     </row>
     <row r="15" spans="1:9" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="76" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="17" spans="2:8" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B17" s="11" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C17" s="67" t="s">
         <v>94</v>
@@ -17421,13 +17466,13 @@
         <v>95</v>
       </c>
       <c r="E17" s="67" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="F17" s="67" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="G17" s="67" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="18" spans="2:8" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -17542,102 +17587,146 @@
     <row r="23" spans="2:8" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B23" s="10"/>
     </row>
-    <row r="82" spans="1:7" ht="15.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="82" spans="1:7" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A82" s="11" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" ht="15.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="F83" s="22" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C83" s="11" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" ht="15.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="85" spans="1:7" ht="15.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F85" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="G83" s="23" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C84" s="95" t="s">
-        <v>109</v>
-      </c>
-      <c r="D84" s="96"/>
-      <c r="E84" s="96"/>
-      <c r="F84" s="102">
+      <c r="G85" s="23" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C86" s="95" t="s">
+        <v>110</v>
+      </c>
+      <c r="D86" s="96"/>
+      <c r="E86" s="96"/>
+      <c r="F86" s="102">
         <v>100</v>
       </c>
-      <c r="G84" s="86">
-        <f>F84/$F$89*100</f>
+      <c r="G86" s="86">
+        <f>F86/$F$91*100</f>
         <v>27.027027027027028</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C85" s="97" t="s">
-        <v>110</v>
-      </c>
-      <c r="D85" s="70"/>
-      <c r="E85" s="70"/>
-      <c r="F85" s="54">
-        <v>80</v>
-      </c>
-      <c r="G85" s="87">
-        <f t="shared" ref="G85:G88" si="0">F85/$F$89*100</f>
-        <v>21.621621621621621</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C86" s="97" t="s">
-        <v>111</v>
-      </c>
-      <c r="D86" s="70"/>
-      <c r="E86" s="70"/>
-      <c r="F86" s="54">
-        <v>80</v>
-      </c>
-      <c r="G86" s="87">
-        <f t="shared" si="0"/>
-        <v>21.621621621621621</v>
       </c>
     </row>
     <row r="87" spans="1:7" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C87" s="97" t="s">
-        <v>91</v>
+        <v>111</v>
       </c>
       <c r="D87" s="70"/>
       <c r="E87" s="70"/>
       <c r="F87" s="54">
+        <v>80</v>
+      </c>
+      <c r="G87" s="87">
+        <f>F87/$F$91*100</f>
+        <v>21.621621621621621</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C88" s="97" t="s">
+        <v>112</v>
+      </c>
+      <c r="D88" s="70"/>
+      <c r="E88" s="70"/>
+      <c r="F88" s="54">
+        <v>80</v>
+      </c>
+      <c r="G88" s="87">
+        <f>F88/$F$91*100</f>
+        <v>21.621621621621621</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C89" s="97" t="s">
+        <v>91</v>
+      </c>
+      <c r="D89" s="70"/>
+      <c r="E89" s="70"/>
+      <c r="F89" s="54">
         <v>60</v>
       </c>
-      <c r="G87" s="87">
-        <f t="shared" si="0"/>
+      <c r="G89" s="87">
+        <f>F89/$F$91*100</f>
         <v>16.216216216216218</v>
       </c>
     </row>
-    <row r="88" spans="1:7" ht="15.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C88" s="98" t="s">
+    <row r="90" spans="1:7" ht="15.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C90" s="98" t="s">
         <v>100</v>
       </c>
-      <c r="D88" s="55"/>
-      <c r="E88" s="55"/>
-      <c r="F88" s="57">
+      <c r="D90" s="55"/>
+      <c r="E90" s="55"/>
+      <c r="F90" s="57">
         <v>50</v>
       </c>
-      <c r="G88" s="88">
-        <f t="shared" si="0"/>
+      <c r="G90" s="88">
+        <f>F90/$F$91*100</f>
         <v>13.513513513513514</v>
       </c>
     </row>
-    <row r="89" spans="1:7" ht="15.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C89" s="99" t="s">
-        <v>126</v>
-      </c>
-      <c r="D89" s="100"/>
-      <c r="E89" s="100"/>
-      <c r="F89" s="103">
-        <f>SUM(F84:F88)</f>
+    <row r="91" spans="1:7" ht="15.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C91" s="99" t="s">
+        <v>129</v>
+      </c>
+      <c r="D91" s="100"/>
+      <c r="E91" s="100"/>
+      <c r="F91" s="103">
+        <f>SUM(F86:F90)</f>
         <v>370</v>
       </c>
-      <c r="G89" s="101">
-        <f>SUM(G84:G88)</f>
+      <c r="G91" s="101">
+        <f>SUM(G86:G90)</f>
         <v>100</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C93" s="11" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" ht="15.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="95" spans="1:7" ht="15.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D95" s="21" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C96" s="102" t="s">
+        <v>135</v>
+      </c>
+      <c r="D96" s="86">
+        <f>G86+G87</f>
+        <v>48.648648648648646</v>
+      </c>
+    </row>
+    <row r="97" spans="3:4" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C97" s="54" t="s">
+        <v>112</v>
+      </c>
+      <c r="D97" s="87">
+        <f>G88</f>
+        <v>21.621621621621621</v>
+      </c>
+    </row>
+    <row r="98" spans="3:4" ht="15.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C98" s="57" t="s">
+        <v>136</v>
+      </c>
+      <c r="D98" s="88">
+        <f>G89+G90</f>
+        <v>29.729729729729733</v>
       </c>
     </row>
   </sheetData>
@@ -17649,20 +17738,226 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB378B99-37B5-4CCF-952B-6B38A828707A}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="5.1640625" customWidth="1"/>
+    <col min="3" max="3" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.9140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.25" customWidth="1"/>
+    <col min="6" max="6" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13" customWidth="1"/>
+    <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A1" s="20" t="s">
-        <v>121</v>
+        <v>124</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" s="11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C5" s="67" t="s">
+        <v>110</v>
+      </c>
+      <c r="D5" s="67" t="s">
+        <v>111</v>
+      </c>
+      <c r="E5" s="67" t="s">
+        <v>112</v>
+      </c>
+      <c r="F5" s="67" t="s">
+        <v>113</v>
+      </c>
+      <c r="G5" s="67" t="s">
+        <v>103</v>
+      </c>
+      <c r="H5" s="15" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C6">
+        <v>50</v>
+      </c>
+      <c r="D6">
+        <v>100</v>
+      </c>
+      <c r="E6">
+        <v>100</v>
+      </c>
+      <c r="F6">
+        <v>100</v>
+      </c>
+      <c r="G6">
+        <v>72</v>
+      </c>
+      <c r="H6" s="13" cm="1">
+        <f t="array" ref="H6">SUMPRODUCT(TRANSPOSE(C6:G6),'Task3 - Value Funcs and Weights'!$G$86:$G$90)/100</f>
+        <v>82.702702702702695</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C7">
+        <v>100</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>25</v>
+      </c>
+      <c r="F7">
+        <v>95</v>
+      </c>
+      <c r="G7">
+        <v>87</v>
+      </c>
+      <c r="H7" s="13" cm="1">
+        <f t="array" ref="H7">SUMPRODUCT(TRANSPOSE(C7:G7),'Task3 - Value Funcs and Weights'!$G$86:$G$90)/100</f>
+        <v>59.594594594594604</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B8" t="s">
+        <v>81</v>
+      </c>
+      <c r="C8">
+        <v>33</v>
+      </c>
+      <c r="D8">
+        <v>67</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>29</v>
+      </c>
+      <c r="H8" s="13" cm="1">
+        <f t="array" ref="H8">SUMPRODUCT(TRANSPOSE(C8:G8),'Task3 - Value Funcs and Weights'!$G$86:$G$90)/100</f>
+        <v>27.324324324324326</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9">
+        <v>17</v>
+      </c>
+      <c r="D9">
+        <v>83</v>
+      </c>
+      <c r="E9">
+        <v>25</v>
+      </c>
+      <c r="F9">
+        <v>35</v>
+      </c>
+      <c r="G9">
+        <v>100</v>
+      </c>
+      <c r="H9" s="13" cm="1">
+        <f t="array" ref="H9">SUMPRODUCT(TRANSPOSE(C9:G9),'Task3 - Value Funcs and Weights'!$G$86:$G$90)/100</f>
+        <v>47.13513513513513</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>83</v>
+      </c>
+      <c r="E10">
+        <v>22</v>
+      </c>
+      <c r="F10">
+        <v>98</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10" s="13" cm="1">
+        <f t="array" ref="H10">SUMPRODUCT(TRANSPOSE(C10:G10),'Task3 - Value Funcs and Weights'!$G$86:$G$90)/100</f>
+        <v>38.594594594594604</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B11" t="s">
+        <v>87</v>
+      </c>
+      <c r="C11">
+        <v>33</v>
+      </c>
+      <c r="D11">
+        <v>50</v>
+      </c>
+      <c r="E11">
+        <v>25</v>
+      </c>
+      <c r="F11">
+        <v>100</v>
+      </c>
+      <c r="G11">
+        <v>33</v>
+      </c>
+      <c r="H11" s="13" cm="1">
+        <f t="array" ref="H11">SUMPRODUCT(TRANSPOSE(C11:G11),'Task3 - Value Funcs and Weights'!$G$86:$G$90)/100</f>
+        <v>45.810810810810807</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A15" s="11"/>
+      <c r="B15" t="s">
+        <v>138</v>
+      </c>
+      <c r="E15" t="str">
+        <f>VLOOKUP(_xlfn.XLOOKUP(MAX(H6:H11),H6:H11,B6:B11),'Task3 - Raw Data'!B6:J11,5)</f>
+        <v>cnr Lygon St, Princes St</v>
+      </c>
+      <c r="G15" t="str">
+        <f>_xlfn.CONCAT("in ",VLOOKUP(E15,'Task3 - Raw Data'!F6:J11,5))</f>
+        <v>in Carlton Nth</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A17" s="11" t="s">
+        <v>141</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>